<commit_message>
đã ổn có thể work với <br>
</commit_message>
<xml_diff>
--- a/test_upload.xlsx
+++ b/test_upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhbaonguyen/Downloads/go-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2436E8-D781-FA49-B053-D6A159114C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4694298-B3D2-A642-B7D3-B30C4E7DCCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18520" yWindow="1800" windowWidth="14700" windowHeight="17440" xr2:uid="{9553992A-8F98-094F-9849-00AEAA0507E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>description</t>
   </si>
@@ -337,6 +337,59 @@
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>dòng 4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in đậm.    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, test.     này là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in      nghiệm.   , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test này là </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>underline</t>
     </r>
   </si>
 </sst>
@@ -777,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BAE912-A59D-4C4C-917C-824EF22A1725}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,7 +900,9 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>

</xml_diff>